<commit_message>
regularExpression_Optimization code Commi Success
</commit_message>
<xml_diff>
--- a/EmployeeDatas.xlsx
+++ b/EmployeeDatas.xlsx
@@ -14,7 +14,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="11" uniqueCount="11">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="20" uniqueCount="17">
   <si>
     <t>Emp ID</t>
   </si>
@@ -40,13 +40,31 @@
     <t>pass</t>
   </si>
   <si>
-    <t>gous</t>
-  </si>
-  <si>
-    <t>gousegmail.com</t>
+    <t>Manish</t>
+  </si>
+  <si>
+    <t>mani@gmail.com</t>
   </si>
   <si>
     <t>fail</t>
+  </si>
+  <si>
+    <t>Dini</t>
+  </si>
+  <si>
+    <t>dini@gmail.com</t>
+  </si>
+  <si>
+    <t>Sanjai</t>
+  </si>
+  <si>
+    <t>sanjaigmail.com</t>
+  </si>
+  <si>
+    <t>gouse</t>
+  </si>
+  <si>
+    <t>gouse@gmail.com</t>
   </si>
 </sst>
 </file>
@@ -54,7 +72,7 @@
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" mc:Ignorable="x14ac">
   <numFmts count="0"/>
-  <fonts count="3" x14ac:knownFonts="1">
+  <fonts count="4" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -72,6 +90,12 @@
       <u/>
       <sz val="11"/>
       <color rgb="FF000000"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color theme="1"/>
       <name val="Calibri"/>
       <family val="2"/>
     </font>
@@ -103,7 +127,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="6">
+  <cellXfs count="7">
     <xf xfId="0" numFmtId="0" borderId="0" fontId="0" fillId="0"/>
     <xf xfId="0" numFmtId="3" applyNumberFormat="1" borderId="1" applyBorder="1" fontId="1" applyFont="1" fillId="0" applyAlignment="1">
       <alignment horizontal="right"/>
@@ -113,6 +137,9 @@
     </xf>
     <xf xfId="0" numFmtId="0" borderId="1" applyBorder="1" fontId="2" applyFont="1" fillId="0" applyAlignment="1">
       <alignment horizontal="left"/>
+    </xf>
+    <xf xfId="0" numFmtId="3" applyNumberFormat="1" borderId="1" applyBorder="1" fontId="3" applyFont="1" fillId="0" applyAlignment="1">
+      <alignment horizontal="right"/>
     </xf>
     <xf xfId="0" numFmtId="3" applyNumberFormat="1" borderId="0" fontId="0" fillId="0" applyAlignment="1">
       <alignment horizontal="right"/>
@@ -422,17 +449,17 @@
   <sheetPr>
     <outlinePr summaryBelow="0"/>
   </sheetPr>
-  <dimension ref="A1:E3"/>
+  <dimension ref="A1:E6"/>
   <sheetViews>
     <sheetView workbookViewId="0" tabSelected="1"/>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" style="4" width="18.14785714285714" customWidth="1" bestFit="1"/>
-    <col min="2" max="2" style="5" width="18.433571428571426" customWidth="1" bestFit="1"/>
-    <col min="3" max="3" style="5" width="26.290714285714284" customWidth="1" bestFit="1"/>
-    <col min="4" max="4" style="4" width="26.433571428571426" customWidth="1" bestFit="1"/>
-    <col min="5" max="5" style="5" width="14.147857142857141" customWidth="1" bestFit="1"/>
+    <col min="1" max="1" style="5" width="18.14785714285714" customWidth="1" bestFit="1"/>
+    <col min="2" max="2" style="6" width="18.433571428571426" customWidth="1" bestFit="1"/>
+    <col min="3" max="3" style="6" width="26.290714285714284" customWidth="1" bestFit="1"/>
+    <col min="4" max="4" style="5" width="26.433571428571426" customWidth="1" bestFit="1"/>
+    <col min="5" max="5" style="6" width="14.147857142857141" customWidth="1" bestFit="1"/>
   </cols>
   <sheetData>
     <row x14ac:dyDescent="0.25" r="1" customHeight="1" ht="19.5">
@@ -471,7 +498,7 @@
     </row>
     <row x14ac:dyDescent="0.25" r="3" customHeight="1" ht="19.5">
       <c r="A3" s="1">
-        <v>765414</v>
+        <v>33571</v>
       </c>
       <c r="B3" s="2" t="s">
         <v>8</v>
@@ -480,9 +507,60 @@
         <v>9</v>
       </c>
       <c r="D3" s="1">
+        <v>8825278234</v>
+      </c>
+      <c r="E3" s="2" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row x14ac:dyDescent="0.25" r="4" customHeight="1" ht="19.5">
+      <c r="A4" s="4">
+        <v>335671</v>
+      </c>
+      <c r="B4" s="2" t="s">
+        <v>11</v>
+      </c>
+      <c r="C4" s="2" t="s">
+        <v>12</v>
+      </c>
+      <c r="D4" s="4">
+        <v>9787362176</v>
+      </c>
+      <c r="E4" s="2" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row x14ac:dyDescent="0.25" r="5" customHeight="1" ht="19.5">
+      <c r="A5" s="4">
+        <v>112418</v>
+      </c>
+      <c r="B5" s="2" t="s">
+        <v>13</v>
+      </c>
+      <c r="C5" s="2" t="s">
+        <v>14</v>
+      </c>
+      <c r="D5" s="4">
+        <v>8976542673</v>
+      </c>
+      <c r="E5" s="2" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row x14ac:dyDescent="0.25" r="6" customHeight="1" ht="19.5">
+      <c r="A6" s="1">
+        <v>765414</v>
+      </c>
+      <c r="B6" s="2" t="s">
+        <v>15</v>
+      </c>
+      <c r="C6" s="2" t="s">
+        <v>16</v>
+      </c>
+      <c r="D6" s="1">
         <v>987654267</v>
       </c>
-      <c r="E3" s="2" t="s">
+      <c r="E6" s="2" t="s">
         <v>10</v>
       </c>
     </row>

</xml_diff>